<commit_message>
Fix bug export + ajout documents de Zied
</commit_message>
<xml_diff>
--- a/Gestion de projet/CD/Dimension Projets/Dossier Projet/PAQL/Dashboard.xlsx
+++ b/Gestion de projet/CD/Dimension Projets/Dossier Projet/PAQL/Dashboard.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Version 1</t>
   </si>
@@ -92,12 +92,15 @@
   <si>
     <t>v4</t>
   </si>
+  <si>
+    <t>v5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +118,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -407,12 +417,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,22 +533,29 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -538,6 +564,90 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,46 +660,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,7 +747,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Résultat de l'algorithme et interface</c:v>
+            <c:v>v1</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dPt>
@@ -720,7 +803,7 @@
                   <c:v>0.79990000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46800000000000003</c:v>
+                  <c:v>0.40029999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.47499999999999998</c:v>
@@ -739,7 +822,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Application minimale</c:v>
+            <c:v>v2</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -752,7 +835,7 @@
                   <c:v>0.74880000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42880000000000001</c:v>
+                  <c:v>0.36940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.51249999999999996</c:v>
@@ -762,6 +845,102 @@
                 </c:pt>
                 <c:pt idx="4" formatCode="0%">
                   <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>v3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$18:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.45350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39689999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$K$18:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.96250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v5</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$18:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.95409999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41410000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94440000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,11 +956,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="146624512"/>
-        <c:axId val="146626048"/>
+        <c:axId val="146626816"/>
+        <c:axId val="146632704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146624512"/>
+        <c:axId val="146626816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,7 +969,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146626048"/>
+        <c:crossAx val="146632704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -798,7 +977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146626048"/>
+        <c:axId val="146632704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +993,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="146624512"/>
+        <c:crossAx val="146626816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -880,7 +1059,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Résultat de l'algorithme et interface</c:v>
+            <c:v>v1</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dPt>
@@ -914,10 +1093,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.64</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -927,7 +1106,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Application minimale</c:v>
+            <c:v>v2</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -937,10 +1116,79 @@
                 <c:formatCode>0,00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.62519999999999998</c:v>
+                  <c:v>0.58550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63290000000000002</c:v>
+                  <c:v>0.58379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>v3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$29:$L$30</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0,00%">
+                  <c:v>0.41820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$M$29:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.75970000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77739999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v5</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$N$29:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,11 +1204,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="146667776"/>
-        <c:axId val="147652608"/>
+        <c:axId val="148446208"/>
+        <c:axId val="148456192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146667776"/>
+        <c:axId val="148446208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +1217,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147652608"/>
+        <c:crossAx val="148456192"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +1225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147652608"/>
+        <c:axId val="148456192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -995,7 +1243,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="146667776"/>
+        <c:crossAx val="148446208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1061,7 +1309,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Résultat de l'algorithme et interface</c:v>
+            <c:v>v1</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1071,7 +1319,7 @@
                 <c:formatCode>0,00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.57372222222222236</c:v>
+                  <c:v>0.55490277777777786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,7 +1329,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Application minimale</c:v>
+            <c:v>v2</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1091,7 +1339,67 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.62186111111111109</c:v>
+                  <c:v>0.61958333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>v3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.50265277777777773</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.77198611111111104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v5</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.79941666666666644</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,11 +1415,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="147673856"/>
-        <c:axId val="147675392"/>
+        <c:axId val="148484096"/>
+        <c:axId val="148485632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147673856"/>
+        <c:axId val="148484096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1428,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147675392"/>
+        <c:crossAx val="148485632"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1128,7 +1436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147675392"/>
+        <c:axId val="148485632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1146,7 +1454,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="147673856"/>
+        <c:crossAx val="148484096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,20 +1476,581 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Evolution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> de la qualité logicielle</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Evolution</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5462668816039986E-17"/>
+                  <c:y val="6.0185185185185182E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>V1; 55,49%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1111111111111112E-2"/>
+                  <c:y val="-6.4814814814814811E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>V2; 62%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7777777777777776E-2"/>
+                  <c:y val="2.7777777777777776E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>V3; 50%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="5.5555555555555552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>V4; 77%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>V5; 80%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$N$5:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0,00%">
+                  <c:v>0.55490000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="149226240"/>
+        <c:axId val="149228928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="149226240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149228928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="149228928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0,00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149226240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>v1</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$D$18:$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Fonctionalité </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Maintenabilité </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fiabilité </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Efficacité</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ergonomie </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$E$18:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.79990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>v2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$18:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.74880000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72219999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>v3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$18:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.45350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39689999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v4</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$K$18:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.96250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v5</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$18:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>0,00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.95409999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41410000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94440000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="151729280"/>
+        <c:axId val="151730816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="151729280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151730816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="151730816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151729280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>90486</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1202,16 +2071,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>809626</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733426</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>447676</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1232,16 +2101,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1255,6 +2124,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Graphique 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1550,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,36 +2495,36 @@
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="88" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61" t="s">
+      <c r="D1" s="62"/>
+      <c r="E1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61" t="s">
+      <c r="J1" s="62"/>
+      <c r="K1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="61"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
+      <c r="L1" s="62"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -1626,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
@@ -1655,94 +2586,116 @@
       <c r="J3" s="39">
         <v>0.92500000000000004</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="39">
+        <v>0.95830000000000004</v>
+      </c>
+      <c r="L3" s="45">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="70">
+      <c r="C4" s="63">
         <v>0.79990000000000006</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="50">
+      <c r="D4" s="64"/>
+      <c r="E4" s="65">
         <v>0.74880000000000002</v>
       </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="66">
+      <c r="F4" s="66"/>
+      <c r="G4" s="67">
         <v>0.45350000000000001</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="66">
+      <c r="H4" s="66"/>
+      <c r="I4" s="67">
         <v>0.96250000000000002</v>
       </c>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="66"/>
+      <c r="K4" s="67">
+        <v>0.95409999999999995</v>
+      </c>
+      <c r="L4" s="66"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="27">
-        <v>0.50760000000000005</v>
+        <v>0.372</v>
       </c>
       <c r="D5" s="28">
         <v>0.42849999999999999</v>
       </c>
       <c r="E5" s="37">
-        <v>0.50049999999999994</v>
+        <v>0.38159999999999999</v>
       </c>
       <c r="F5" s="36">
         <v>0.35709999999999997</v>
       </c>
       <c r="G5" s="39">
-        <v>0.34260000000000002</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="H5" s="39">
         <v>0.39279999999999998</v>
       </c>
       <c r="I5" s="39">
-        <v>0.35399999999999998</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="J5" s="39">
         <v>0.42849999999999999</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="39">
+        <v>0.39979999999999999</v>
+      </c>
+      <c r="L5" s="39">
+        <v>0.42849999999999999</v>
+      </c>
+      <c r="N5" s="51">
+        <v>0.55490000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="63">
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="65">
-        <v>0.42880000000000001</v>
-      </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49">
-        <v>0.36770000000000003</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49">
-        <v>0.39119999999999999</v>
-      </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="48"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="92">
+        <f>(C5+D5)/2</f>
+        <v>0.40024999999999999</v>
+      </c>
+      <c r="D6" s="93"/>
+      <c r="E6" s="94">
+        <f>(E5+F5)/2</f>
+        <v>0.36934999999999996</v>
+      </c>
+      <c r="F6" s="69"/>
+      <c r="G6" s="68">
+        <f>(G5+H5)/2</f>
+        <v>0.39690000000000003</v>
+      </c>
+      <c r="H6" s="69"/>
+      <c r="I6" s="68">
+        <f>(I5+J5)/2</f>
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="J6" s="69"/>
+      <c r="K6" s="68">
+        <v>0.41410000000000002</v>
+      </c>
+      <c r="L6" s="69"/>
+      <c r="N6" s="52">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
@@ -1771,10 +2724,17 @@
       <c r="J7" s="45">
         <v>0.8</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="L7" s="45">
+        <v>1</v>
+      </c>
+      <c r="N7" s="53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
@@ -1784,23 +2744,28 @@
       <c r="C8" s="70">
         <v>0.47499999999999998</v>
       </c>
-      <c r="D8" s="68"/>
-      <c r="E8" s="50">
+      <c r="D8" s="71"/>
+      <c r="E8" s="72">
         <v>0.51249999999999996</v>
       </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="66">
+      <c r="F8" s="73"/>
+      <c r="G8" s="74">
         <v>0.42499999999999999</v>
       </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="66">
+      <c r="H8" s="73"/>
+      <c r="I8" s="74">
         <v>0.83750000000000002</v>
       </c>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="73"/>
+      <c r="K8" s="74">
+        <v>0.875</v>
+      </c>
+      <c r="L8" s="73"/>
+      <c r="N8" s="52">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1822,35 +2787,43 @@
         <v>0.83330000000000004</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="39">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="N9" s="52">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="22">
         <v>0.5</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="77">
         <v>0.5</v>
       </c>
-      <c r="D10" s="68"/>
-      <c r="E10" s="50">
+      <c r="D10" s="78"/>
+      <c r="E10" s="84">
         <v>0.72219999999999995</v>
       </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="66">
+      <c r="F10" s="85"/>
+      <c r="G10" s="86">
         <v>0.33329999999999999</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="66">
+      <c r="H10" s="85"/>
+      <c r="I10" s="86">
         <v>0.83330000000000004</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="85"/>
+      <c r="K10" s="86">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="L10" s="85"/>
+      <c r="N10" s="54"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
@@ -1872,35 +2845,40 @@
         <v>0.9</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="45">
+        <v>0.95</v>
+      </c>
+      <c r="N11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="24">
         <v>1</v>
       </c>
-      <c r="C12" s="67">
+      <c r="C12" s="79">
         <v>0.5</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="52">
+      <c r="D12" s="80"/>
+      <c r="E12" s="81">
         <v>0.7</v>
       </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="69">
+      <c r="F12" s="82"/>
+      <c r="G12" s="83">
         <v>0.75</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="69">
+      <c r="H12" s="82"/>
+      <c r="I12" s="83">
         <v>0.9</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="82"/>
+      <c r="K12" s="83">
+        <v>0.95</v>
+      </c>
+      <c r="L12" s="82"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="9"/>
       <c r="C13" s="5"/>
@@ -1914,223 +2892,263 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="32">
-        <f>(C3*B4+C5*B6+C7*B8)/2.1</f>
-        <v>0.64247619047619042</v>
+        <f>(C3+C5+C7)/3</f>
+        <v>0.62953333333333328</v>
       </c>
       <c r="D14" s="33">
-        <f>(D3+D5+D7*B8+D9*B10+D11*B12)/3.6</f>
-        <v>0.56438888888888894</v>
+        <f>(D3+D5+D7+D9+D11)/5</f>
+        <v>0.49236000000000002</v>
       </c>
       <c r="E14" s="38">
-        <v>0.62519999999999998</v>
+        <v>0.58550000000000002</v>
       </c>
       <c r="F14" s="39">
-        <v>0.63290000000000002</v>
+        <v>0.58379999999999999</v>
       </c>
       <c r="G14" s="39">
-        <v>0.3987</v>
+        <f>(G3+G5+G7)/3</f>
+        <v>0.41816666666666674</v>
       </c>
       <c r="H14" s="46">
         <f>(H3+H5+H7+H9+H11)/5</f>
         <v>0.47592000000000001</v>
       </c>
       <c r="I14" s="39">
-        <v>0.74299999999999999</v>
+        <f>(I3+I5+I7)/3</f>
+        <v>0.7596666666666666</v>
       </c>
       <c r="J14" s="39">
-        <v>0.77729999999999999</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>(J3+J5+J7+J9+J11)/5</f>
+        <v>0.77736000000000005</v>
+      </c>
+      <c r="K14" s="46">
+        <f>(K3+K5+K7)/3</f>
+        <v>0.7027000000000001</v>
+      </c>
+      <c r="L14" s="46">
+        <f>(L3+L5+L7+L9+L11)/5</f>
+        <v>0.85458000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="57">
+      <c r="C15" s="90">
         <f>(C4*B4+C6*B6+C8*B8+C10*B10+C12*B12)/3.6</f>
-        <v>0.57372222222222236</v>
-      </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59">
-        <f>((E8*0)+(E10*0.5)+E4+E6+E12)/3.6</f>
-        <v>0.62186111111111109</v>
-      </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="59">
+        <v>0.55490277777777786</v>
+      </c>
+      <c r="D15" s="91"/>
+      <c r="E15" s="75">
+        <f>((E8*0.1)+(E10*0.5)+E4+E6+E12)/3.6</f>
+        <v>0.61958333333333337</v>
+      </c>
+      <c r="F15" s="76"/>
+      <c r="G15" s="75">
         <f>((G8*0.1)+(G10*0.5)+G4+G6+G12)/3.6</f>
-        <v>0.4945416666666666</v>
-      </c>
-      <c r="H15" s="60"/>
-      <c r="I15" s="59">
+        <v>0.50265277777777773</v>
+      </c>
+      <c r="H15" s="76"/>
+      <c r="I15" s="75">
         <f>((I8*0.1)+(I10*0.5)+I4+I6+I12)/3.6</f>
-        <v>0.76502777777777786</v>
-      </c>
-      <c r="J15" s="60"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="48"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.77198611111111104</v>
+      </c>
+      <c r="J15" s="76"/>
+      <c r="K15" s="75">
+        <f>((K8*0.1)+(K10*0.5)+K4+K6+K12)/3.6</f>
+        <v>0.79941666666666644</v>
+      </c>
+      <c r="L15" s="76"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="9"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="9"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62" t="s">
+      <c r="F17" s="55"/>
+      <c r="G17" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="47" t="s">
+      <c r="H17" s="55"/>
+      <c r="I17" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="48"/>
+      <c r="J17" s="57"/>
       <c r="K17" s="44" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="58">
         <v>0.79990000000000006</v>
       </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="49">
+      <c r="F18" s="59"/>
+      <c r="G18" s="56">
         <v>0.74880000000000002</v>
       </c>
-      <c r="H18" s="48"/>
-      <c r="I18" s="49">
+      <c r="H18" s="57"/>
+      <c r="I18" s="56">
         <v>0.45350000000000001</v>
       </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="96"/>
+      <c r="K18" s="39">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="L18" s="48">
+        <v>0.95409999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="54">
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="F19" s="71"/>
-      <c r="G19" s="49">
-        <v>0.42880000000000001</v>
-      </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49">
-        <v>0.36770000000000003</v>
-      </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="59">
+        <v>0.40029999999999999</v>
+      </c>
+      <c r="F19" s="60"/>
+      <c r="G19" s="56">
+        <v>0.36940000000000001</v>
+      </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="56">
+        <v>0.39689999999999998</v>
+      </c>
+      <c r="J19" s="96"/>
+      <c r="K19" s="39">
+        <v>0.4163</v>
+      </c>
+      <c r="L19" s="48">
+        <v>0.41410000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="58">
         <v>0.47499999999999998</v>
       </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="49">
+      <c r="F20" s="59"/>
+      <c r="G20" s="56">
         <v>0.51249999999999996</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="49">
+      <c r="H20" s="57"/>
+      <c r="I20" s="56">
         <v>0.42499999999999999</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="96"/>
+      <c r="K20" s="39">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="L20" s="48">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="9"/>
       <c r="C21" s="5"/>
       <c r="D21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="53">
+      <c r="E21" s="58">
         <v>0.5</v>
       </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="49">
+      <c r="F21" s="59"/>
+      <c r="G21" s="56">
         <v>0.72219999999999995</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="49">
+      <c r="H21" s="57"/>
+      <c r="I21" s="56">
         <v>0.33329999999999999</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="96"/>
+      <c r="K21" s="39">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="L21" s="48">
+        <v>0.94440000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="9"/>
       <c r="C22" s="5"/>
       <c r="D22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="53">
+      <c r="E22" s="58">
         <v>0.5</v>
       </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="51">
+      <c r="F22" s="59"/>
+      <c r="G22" s="61">
         <v>0.7</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="51">
+      <c r="H22" s="57"/>
+      <c r="I22" s="61">
         <v>0.75</v>
       </c>
-      <c r="J22" s="52"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J22" s="87"/>
+      <c r="K22" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="L22" s="49">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="9"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="9"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="9"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="9"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="9"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="9"/>
       <c r="C28" s="5"/>
@@ -2145,11 +3163,14 @@
       <c r="L28" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="M28" s="72" t="s">
+      <c r="M28" s="50" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="9"/>
       <c r="C29" s="5"/>
@@ -2158,30 +3179,40 @@
         <v>17</v>
       </c>
       <c r="J29" s="34">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="K29" s="36">
-        <v>0.62519999999999998</v>
-      </c>
-      <c r="L29" s="43">
-        <v>39.869999999999997</v>
-      </c>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.58550000000000002</v>
+      </c>
+      <c r="L29" s="48">
+        <v>0.41820000000000002</v>
+      </c>
+      <c r="M29" s="39">
+        <v>0.75970000000000004</v>
+      </c>
+      <c r="N29" s="45">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I30" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J30" s="34">
-        <v>0.56000000000000005</v>
+        <v>0.49</v>
       </c>
       <c r="K30" s="36">
-        <v>0.63290000000000002</v>
+        <v>0.58379999999999999</v>
       </c>
       <c r="L30" s="34">
         <v>0.48</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="39">
+        <v>0.77739999999999998</v>
+      </c>
+      <c r="N30" s="45">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" s="5"/>
@@ -2227,13 +3258,37 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="K1:L1"/>
@@ -2250,37 +3305,13 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>